<commit_message>
Code to Variable excel
</commit_message>
<xml_diff>
--- a/VarCode_Meaning.xlsx
+++ b/VarCode_Meaning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabhjain/git/NLSY97-Analysis-R-Prog-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8E3447-5487-1843-9354-74D09A9FC28C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2132DB-4A08-DA43-B70B-CA128D72CAF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{B7924913-9FA0-D544-B0ED-6E1D27225704}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
   <si>
     <t>U1852400</t>
   </si>
@@ -244,6 +244,36 @@
   </si>
   <si>
     <t>debt.30</t>
+  </si>
+  <si>
+    <t>WHAT IS CURRENT HIGHEST GRADE EVER COMPLETED? 2011</t>
+  </si>
+  <si>
+    <t>U1718000</t>
+  </si>
+  <si>
+    <t>TYPE OF BUS OR INDUSTRY CODE (2002 CENSUS 4-DIGIT)</t>
+  </si>
+  <si>
+    <t>PERCENT CHANCE R HAS COLLEGE DEGREE BY 30 YEARS OLD 1997</t>
+  </si>
+  <si>
+    <t>U1719400</t>
+  </si>
+  <si>
+    <t>OCCUPATION/JOB CODE (2002 CENSUS 4-DIGIT) 2017</t>
+  </si>
+  <si>
+    <t>high.grade.completed.11</t>
+  </si>
+  <si>
+    <t>type.business</t>
+  </si>
+  <si>
+    <t>pct.college.30.1997</t>
+  </si>
+  <si>
+    <t>occupation</t>
   </si>
 </sst>
 </file>
@@ -595,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85166C1-D365-1240-AC96-24F603B18A8D}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,6 +913,50 @@
         <v>72</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>